<commit_message>
rename metadata columns for gross checks
</commit_message>
<xml_diff>
--- a/inst/extdata/ExampleMeta.xlsx
+++ b/inst/extdata/ExampleMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\AquaSensR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD765E66-9640-46C3-B8D3-0134E8DD13E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FAB42F-B0F4-411D-91EE-9636581D8650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32460" yWindow="825" windowWidth="18270" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,6 @@
     <t>Depth</t>
   </si>
   <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Tlower</t>
-  </si>
-  <si>
-    <t>Tupper</t>
-  </si>
-  <si>
     <t>SpikeFail</t>
   </si>
   <si>
@@ -89,6 +77,18 @@
   </si>
   <si>
     <t>Salinity_ppt</t>
+  </si>
+  <si>
+    <t>GrMinFail</t>
+  </si>
+  <si>
+    <t>GrMaxFail</t>
+  </si>
+  <si>
+    <t>GrMinSuspect</t>
+  </si>
+  <si>
+    <t>GrMaxSuspect</t>
   </si>
 </sst>
 </file>
@@ -444,12 +444,26 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -463,60 +477,60 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>-0.5</v>
       </c>
       <c r="G2">
-        <v>28.3</v>
+        <v>25</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -545,19 +559,22 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D3">
+        <v>-1</v>
+      </c>
+      <c r="E3">
+        <v>120</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>150</v>
-      </c>
-      <c r="F3">
-        <v>60</v>
+      <c r="G3">
+        <v>100</v>
       </c>
       <c r="H3">
         <v>25</v>
@@ -586,19 +603,22 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
       </c>
       <c r="H4">
         <v>4</v>
@@ -627,16 +647,22 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>1000</v>
+        <v>1500</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>1200</v>
       </c>
       <c r="H5">
         <v>10</v>
@@ -665,16 +691,22 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>1000</v>
+        <v>1500</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>1200</v>
       </c>
       <c r="H6">
         <v>100</v>
@@ -703,16 +735,22 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>37</v>
       </c>
       <c r="H7">
         <v>5</v>
@@ -741,22 +779,22 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
       <c r="D8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>8.3000000000000007</v>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>10</v>

</xml_diff>